<commit_message>
fix(bulk-import): delete categories for persons and add researchgate to mapping
</commit_message>
<xml_diff>
--- a/src/components/bulk-imports/xlsx-test/persons.xlsx
+++ b/src/components/bulk-imports/xlsx-test/persons.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t xml:space="preserve">Prénom</t>
   </si>
@@ -31,19 +31,28 @@
     <t xml:space="preserve">Genre [F = Femme, H = Homme, A = Autre]</t>
   </si>
   <si>
+    <t xml:space="preserve">Autres dénominations possibles séparées par des ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifiant Orcid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identifiant Wikidata [Q1234]</t>
   </si>
   <si>
     <t xml:space="preserve">Identifiant IdRef [123456789]</t>
   </si>
   <si>
-    <t xml:space="preserve">Activité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date de naissance {1990-05-21}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifiant Orcid</t>
+    <t xml:space="preserve">Site internet en français</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site internet en anglais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compte researchgate [https://researchgate.com/XXX]</t>
   </si>
   <si>
     <t xml:space="preserve">Compte twitter [https://twitter.com/XXX]</t>
@@ -52,9 +61,6 @@
     <t xml:space="preserve">Compte linkedIn [https://www.linkedin.com/in/XXX-XXX-123456/]</t>
   </si>
   <si>
-    <t xml:space="preserve">Dans la recherche publique ? [O : Oui, N : Non]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jean-Luc</t>
   </si>
   <si>
@@ -64,33 +70,30 @@
     <t xml:space="preserve">H</t>
   </si>
   <si>
+    <t xml:space="preserve">Coucou</t>
+  </si>
+  <si>
     <t xml:space="preserve">050643592</t>
   </si>
   <si>
-    <t xml:space="preserve">Coucou</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://twitter.com/mihoub</t>
   </si>
   <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
     <t xml:space="preserve">Michel</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
+    <t xml:space="preserve">Acteur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q102110688</t>
   </si>
   <si>
     <t xml:space="preserve">056180748</t>
   </si>
   <si>
-    <t xml:space="preserve">Acteur</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.linkedin.com/in/cristina-ghitulica-ab5987221/</t>
   </si>
   <si>
@@ -115,12 +118,12 @@
     <t xml:space="preserve">Z</t>
   </si>
   <si>
+    <t xml:space="preserve">Agent de la maréchaussée</t>
+  </si>
+  <si>
     <t xml:space="preserve">119922851</t>
   </si>
   <si>
-    <t xml:space="preserve">Agent de la maréchaussée</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hélène</t>
   </si>
   <si>
@@ -142,16 +145,16 @@
     <t xml:space="preserve">Sylvain</t>
   </si>
   <si>
-    <t xml:space="preserve">Fe !rez</t>
+    <t xml:space="preserve">Ferez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123123X</t>
   </si>
   <si>
     <t xml:space="preserve">Q58147673</t>
   </si>
   <si>
     <t xml:space="preserve">080146813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123123X</t>
   </si>
   <si>
     <t xml:space="preserve">Foulloy</t>
@@ -168,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -198,12 +201,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -266,24 +263,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -367,27 +364,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:J"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="62.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="56.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="73"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -397,7 +395,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -421,388 +419,437 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="n">
-        <v>33014</v>
-      </c>
-      <c r="H2" s="6" t="n">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="n">
         <v>1231233</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>17</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5" t="n">
-        <v>33014</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7" t="n">
+        <v>12312</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5" t="n">
-        <v>33015</v>
-      </c>
-      <c r="H4" s="6" t="n">
-        <v>12312</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6" t="n">
+      <c r="F5" s="7" t="n">
         <v>1231233</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="H5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5" t="n">
-        <v>33017</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>17</v>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="5" t="n">
-        <v>33018</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>17</v>
+      <c r="M7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="F8" s="7" t="n">
         <v>1231233</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>17</v>
+      <c r="M8" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>33020</v>
+      <c r="G9" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="4"/>
-      <c r="K10" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="3"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="3"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="3"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="3"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="https://twitter.com/mihoub"/>
-    <hyperlink ref="I6" r:id="rId2" display="https://twitter.com/mihoub"/>
-    <hyperlink ref="I8" r:id="rId3" display="https://twitter.com/fred"/>
+    <hyperlink ref="K1" r:id="rId1" display="https://researchgate.com/XXX"/>
+    <hyperlink ref="L2" r:id="rId2" display="https://twitter.com/mihoub"/>
+    <hyperlink ref="L6" r:id="rId3" display="https://twitter.com/mihoub"/>
+    <hyperlink ref="L8" r:id="rId4" display="https://twitter.com/fred"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
refactor(regexp): move regexp for identifiers in utils and add orcid regexp
</commit_message>
<xml_diff>
--- a/src/components/bulk-imports/xlsx-test/persons.xlsx
+++ b/src/components/bulk-imports/xlsx-test/persons.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t xml:space="preserve">Prénom</t>
   </si>
@@ -70,12 +70,21 @@
     <t xml:space="preserve">H</t>
   </si>
   <si>
+    <t xml:space="preserve">michelle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coucou</t>
   </si>
   <si>
+    <t xml:space="preserve">Q102110688</t>
+  </si>
+  <si>
     <t xml:space="preserve">050643592</t>
   </si>
   <si>
+    <t xml:space="preserve">https://researchgate.com/mihoub</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://twitter.com/mihoub</t>
   </si>
   <si>
@@ -88,10 +97,10 @@
     <t xml:space="preserve">Acteur</t>
   </si>
   <si>
-    <t xml:space="preserve">Q102110688</t>
-  </si>
-  <si>
     <t xml:space="preserve">056180748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boucoual</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.linkedin.com/in/cristina-ghitulica-ab5987221/</t>
@@ -250,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,7 +272,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,10 +286,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -366,8 +371,8 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:J"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,8 +385,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="34.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="22.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="34.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="47.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="34.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="73"/>
   </cols>
   <sheetData>
@@ -436,184 +442,193 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>1231233</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="M3" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="7" t="n">
+      <c r="F4" s="3" t="n">
         <v>12312</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
       <c r="L4" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="7" t="n">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>1231233</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="3" t="n">
         <v>1231233</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="8" t="n">
+        <v>44</v>
+      </c>
+      <c r="C9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
@@ -622,7 +637,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="H10" s="6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -846,10 +861,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K1" r:id="rId1" display="https://researchgate.com/XXX"/>
-    <hyperlink ref="L2" r:id="rId2" display="https://twitter.com/mihoub"/>
-    <hyperlink ref="L6" r:id="rId3" display="https://twitter.com/mihoub"/>
-    <hyperlink ref="L8" r:id="rId4" display="https://twitter.com/fred"/>
+    <hyperlink ref="K1" r:id="rId1" display="Compte researchgate [https://researchgate.com/XXX]"/>
+    <hyperlink ref="K2" r:id="rId2" display="https://researchgate"/>
+    <hyperlink ref="L2" r:id="rId3" display="https://twitter.com/mihoub"/>
+    <hyperlink ref="L6" r:id="rId4" display="https://twitter.com/mihoub"/>
+    <hyperlink ref="L8" r:id="rId5" display="https://twitter.com/fred"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>